<commit_message>
RSCT: best performance for the FPGA
</commit_message>
<xml_diff>
--- a/fpga-results.xlsx
+++ b/fpga-results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjt/Work/FPGA_CPU_HARP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjt/Work/fpga_cpu_harp2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5EEACD-95BA-4246-8207-B43D127C8B2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D232D2-66B4-8742-B6C1-A9CF37874AD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="540" windowWidth="18160" windowHeight="16140" tabRatio="988" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="400" yWindow="480" windowWidth="18160" windowHeight="16140" tabRatio="988" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RSCD" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Kernel</t>
   </si>
@@ -249,10 +249,6 @@
   </si>
   <si>
     <t>2,191 / 2,713 ( 81 % )</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>r3-1_ul7m_ul2</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -364,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -417,6 +413,7 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1235,15 +1232,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9443AD-ABD6-ED45-8376-5BDE43EC0984}">
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" ht="12">
@@ -1356,56 +1355,56 @@
       </c>
       <c r="Q3" s="11"/>
     </row>
-    <row r="4" spans="1:18" s="14" customFormat="1" ht="36">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:18" s="20" customFormat="1" ht="48">
+      <c r="A4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="16">
         <v>293518</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="17">
         <v>379819</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="18">
         <v>190.625</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="16">
         <v>0.71299999999999997</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="16">
         <v>3.8540000000000001</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="16">
         <v>0.123</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="16">
         <v>2.7429999999999999</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="16">
         <v>1.0109999999999999</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="16">
         <v>1.7310000000000001</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="16">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="16">
         <v>0.95699999999999996</v>
       </c>
-      <c r="Q4" s="11"/>
+      <c r="Q4" s="16"/>
     </row>
     <row r="5" spans="1:18" ht="36">
       <c r="A5" s="2" t="s">
@@ -1458,76 +1457,75 @@
       </c>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" ht="36">
       <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="11">
+        <v>282389</v>
+      </c>
+      <c r="C6" s="12">
+        <v>348624</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" ht="36">
-      <c r="A7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="11">
-        <v>282389</v>
-      </c>
-      <c r="C7" s="12">
-        <v>348624</v>
-      </c>
-      <c r="D7" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="13">
+      <c r="H6" s="13">
         <v>208.33333334</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I6" s="13">
         <v>0.47099999999999997</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J6" s="11">
         <v>3.8719999999999999</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K6" s="11">
         <v>0.123</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L6" s="11">
         <v>2.601</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M6" s="11">
         <v>0.77600000000000002</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N6" s="11">
         <v>1.825</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O6" s="11">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P6" s="11">
         <v>1.0469999999999999</v>
       </c>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="2"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="2"/>
     </row>
@@ -1859,7 +1857,7 @@
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="13"/>
+      <c r="H24" s="11"/>
       <c r="I24" s="13"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
@@ -2151,26 +2149,6 @@
       <c r="Q38" s="11"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="1:18">
-      <c r="A39" s="2"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="2"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>